<commit_message>
Subido por Jorge Alcantara a las 11 p.m
</commit_message>
<xml_diff>
--- a/Tracking_tareas.xlsx
+++ b/Tracking_tareas.xlsx
@@ -128,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,14 +152,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -208,13 +200,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,7 +513,7 @@
   <dimension ref="B2:J20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -536,11 +527,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -848,7 +839,7 @@
       <c r="F14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="4">
@@ -912,8 +903,12 @@
       <c r="H16" s="4">
         <v>40868</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="4">
+        <v>40886</v>
+      </c>
+      <c r="J16" s="4">
+        <v>40886</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
@@ -937,8 +932,12 @@
       <c r="H17" s="4">
         <v>40868</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="4">
+        <v>40886</v>
+      </c>
+      <c r="J17" s="4">
+        <v>40886</v>
+      </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
@@ -962,8 +961,12 @@
       <c r="H18" s="4">
         <v>40868</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="4">
+        <v>40884</v>
+      </c>
+      <c r="J18" s="4">
+        <v>40886</v>
+      </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
@@ -987,8 +990,12 @@
       <c r="H19" s="4">
         <v>40868</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="4">
+        <v>40884</v>
+      </c>
+      <c r="J19" s="4">
+        <v>40886</v>
+      </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
@@ -1012,8 +1019,12 @@
       <c r="H20" s="4">
         <v>40868</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="4">
+        <v>40884</v>
+      </c>
+      <c r="J20" s="4">
+        <v>40886</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>